<commit_message>
prasadk the bug hunter
</commit_message>
<xml_diff>
--- a/PtronN/src/test/resources/testdata.xlsx
+++ b/PtronN/src/test/resources/testdata.xlsx
@@ -8,21 +8,23 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\IT\Selenium Webriver\FrameWork\Backup\PtronN\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{446C2530-5D83-4977-9680-33F5227C5B6A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A9ABD1D-25E3-47EA-8C4F-3F43484B3A96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="13056" firstSheet="6" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="13056" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="validation" sheetId="1" r:id="rId1"/>
-    <sheet name="campaign" sheetId="2" r:id="rId2"/>
-    <sheet name="lead" sheetId="3" r:id="rId3"/>
-    <sheet name="contact" sheetId="5" r:id="rId4"/>
-    <sheet name="potential" sheetId="4" r:id="rId5"/>
-    <sheet name="account" sheetId="6" r:id="rId6"/>
-    <sheet name="purchaseorder" sheetId="7" r:id="rId7"/>
-    <sheet name="vendor" sheetId="8" r:id="rId8"/>
-    <sheet name="product" sheetId="9" r:id="rId9"/>
-    <sheet name="invoice" sheetId="10" r:id="rId10"/>
+    <sheet name="salesorder" sheetId="11" r:id="rId1"/>
+    <sheet name="pricebook" sheetId="12" r:id="rId2"/>
+    <sheet name="validation" sheetId="1" r:id="rId3"/>
+    <sheet name="campaign" sheetId="2" r:id="rId4"/>
+    <sheet name="lead" sheetId="3" r:id="rId5"/>
+    <sheet name="contact" sheetId="5" r:id="rId6"/>
+    <sheet name="potential" sheetId="4" r:id="rId7"/>
+    <sheet name="account" sheetId="6" r:id="rId8"/>
+    <sheet name="purchaseorder" sheetId="7" r:id="rId9"/>
+    <sheet name="vendor" sheetId="8" r:id="rId10"/>
+    <sheet name="product" sheetId="9" r:id="rId11"/>
+    <sheet name="invoice" sheetId="10" r:id="rId12"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2166" uniqueCount="830">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2178" uniqueCount="839">
   <si>
     <t>password</t>
   </si>
@@ -2524,6 +2526,33 @@
   </si>
   <si>
     <t>SONY PLAYSTATION</t>
+  </si>
+  <si>
+    <t>AccnName</t>
+  </si>
+  <si>
+    <t>ProdName</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>SalesOrder</t>
+  </si>
+  <si>
+    <t>Abhay</t>
+  </si>
+  <si>
+    <t>Iphone</t>
+  </si>
+  <si>
+    <t>58999</t>
+  </si>
+  <si>
+    <t>pbname</t>
+  </si>
+  <si>
+    <t>sony</t>
   </si>
 </sst>
 </file>
@@ -2893,6 +2922,346 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B724D644-6C74-4275-886A-D1C414882E61}">
+  <dimension ref="A1:E2"/>
+  <sheetViews>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>768</v>
+      </c>
+      <c r="B1" t="s">
+        <v>830</v>
+      </c>
+      <c r="C1" t="s">
+        <v>831</v>
+      </c>
+      <c r="D1" t="s">
+        <v>832</v>
+      </c>
+      <c r="E1" t="s">
+        <v>771</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>833</v>
+      </c>
+      <c r="B2" t="s">
+        <v>834</v>
+      </c>
+      <c r="C2" t="s">
+        <v>835</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>836</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA4DC77-DCE0-4510-877A-8E54DEB3D6DB}">
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="18.5546875" customWidth="1"/>
+    <col min="5" max="5" width="16.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>788</v>
+      </c>
+      <c r="B1" t="s">
+        <v>787</v>
+      </c>
+      <c r="C1" t="s">
+        <v>786</v>
+      </c>
+      <c r="D1" t="s">
+        <v>785</v>
+      </c>
+      <c r="E1" t="s">
+        <v>784</v>
+      </c>
+      <c r="F1" t="s">
+        <v>783</v>
+      </c>
+      <c r="G1" t="s">
+        <v>737</v>
+      </c>
+      <c r="H1" t="s">
+        <v>736</v>
+      </c>
+      <c r="I1" t="s">
+        <v>739</v>
+      </c>
+      <c r="J1" t="s">
+        <v>738</v>
+      </c>
+      <c r="K1" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>790</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>789</v>
+      </c>
+      <c r="C2" t="s">
+        <v>791</v>
+      </c>
+      <c r="D2" t="s">
+        <v>792</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>793</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>727</v>
+      </c>
+      <c r="G2" t="s">
+        <v>794</v>
+      </c>
+      <c r="H2" t="s">
+        <v>795</v>
+      </c>
+      <c r="I2" t="s">
+        <v>767</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>748</v>
+      </c>
+      <c r="K2" t="s">
+        <v>796</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{157F74EF-AF50-4C9A-AD23-03F5C2C7CA5B}"/>
+    <hyperlink ref="E2" r:id="rId2" xr:uid="{7C8979B8-4FCF-425E-889B-F1634B71312D}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CDAA5F6-59A5-46C2-91A2-2AB506189DA3}">
+  <dimension ref="A1:N2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="6" max="6" width="12.109375" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
+    <col min="8" max="8" width="13.77734375" customWidth="1"/>
+    <col min="9" max="9" width="14.109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>798</v>
+      </c>
+      <c r="B1" t="s">
+        <v>797</v>
+      </c>
+      <c r="C1" t="s">
+        <v>799</v>
+      </c>
+      <c r="D1" t="s">
+        <v>800</v>
+      </c>
+      <c r="E1" t="s">
+        <v>801</v>
+      </c>
+      <c r="F1" t="s">
+        <v>802</v>
+      </c>
+      <c r="G1" t="s">
+        <v>803</v>
+      </c>
+      <c r="H1" t="s">
+        <v>804</v>
+      </c>
+      <c r="I1" t="s">
+        <v>805</v>
+      </c>
+      <c r="J1" t="s">
+        <v>806</v>
+      </c>
+      <c r="K1" t="s">
+        <v>807</v>
+      </c>
+      <c r="L1" t="s">
+        <v>808</v>
+      </c>
+      <c r="M1" t="s">
+        <v>809</v>
+      </c>
+      <c r="N1" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>810</v>
+      </c>
+      <c r="B2" t="s">
+        <v>811</v>
+      </c>
+      <c r="C2" t="s">
+        <v>774</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>684</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>696</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>819</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>818</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>812</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>813</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>814</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>683</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>815</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="N2" t="s">
+        <v>817</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55270884-F8D9-4DEB-81BF-3472001DB335}">
+  <dimension ref="A1:G2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="17.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>820</v>
+      </c>
+      <c r="B1" t="s">
+        <v>821</v>
+      </c>
+      <c r="C1" t="s">
+        <v>797</v>
+      </c>
+      <c r="D1" t="s">
+        <v>772</v>
+      </c>
+      <c r="E1" t="s">
+        <v>822</v>
+      </c>
+      <c r="F1" t="s">
+        <v>823</v>
+      </c>
+      <c r="G1" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>824</v>
+      </c>
+      <c r="B2" t="s">
+        <v>828</v>
+      </c>
+      <c r="C2" t="s">
+        <v>829</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>827</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>688</v>
+      </c>
+      <c r="F2" t="s">
+        <v>825</v>
+      </c>
+      <c r="G2" t="s">
+        <v>826</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F63E0C2-DB0F-4F82-AD2C-E25423915363}">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>837</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>838</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C657"/>
   <sheetViews>
@@ -10141,71 +10510,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{55270884-F8D9-4DEB-81BF-3472001DB335}">
-  <dimension ref="A1:G2"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="17.21875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>820</v>
-      </c>
-      <c r="B1" t="s">
-        <v>821</v>
-      </c>
-      <c r="C1" t="s">
-        <v>797</v>
-      </c>
-      <c r="D1" t="s">
-        <v>772</v>
-      </c>
-      <c r="E1" t="s">
-        <v>822</v>
-      </c>
-      <c r="F1" t="s">
-        <v>823</v>
-      </c>
-      <c r="G1" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>824</v>
-      </c>
-      <c r="B2" t="s">
-        <v>828</v>
-      </c>
-      <c r="C2" t="s">
-        <v>829</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>827</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>688</v>
-      </c>
-      <c r="F2" t="s">
-        <v>825</v>
-      </c>
-      <c r="G2" t="s">
-        <v>826</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K3"/>
   <sheetViews>
@@ -10332,7 +10637,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:M2"/>
   <sheetViews>
@@ -10432,7 +10737,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:K2"/>
   <sheetViews>
@@ -10520,7 +10825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
@@ -10579,7 +10884,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
@@ -10656,7 +10961,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:J2"/>
   <sheetViews>
@@ -10742,206 +11047,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CCA4DC77-DCE0-4510-877A-8E54DEB3D6DB}">
-  <dimension ref="A1:K2"/>
-  <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="2" max="2" width="18.5546875" customWidth="1"/>
-    <col min="5" max="5" width="16.88671875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>788</v>
-      </c>
-      <c r="B1" t="s">
-        <v>787</v>
-      </c>
-      <c r="C1" t="s">
-        <v>786</v>
-      </c>
-      <c r="D1" t="s">
-        <v>785</v>
-      </c>
-      <c r="E1" t="s">
-        <v>784</v>
-      </c>
-      <c r="F1" t="s">
-        <v>783</v>
-      </c>
-      <c r="G1" t="s">
-        <v>737</v>
-      </c>
-      <c r="H1" t="s">
-        <v>736</v>
-      </c>
-      <c r="I1" t="s">
-        <v>739</v>
-      </c>
-      <c r="J1" t="s">
-        <v>738</v>
-      </c>
-      <c r="K1" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>790</v>
-      </c>
-      <c r="B2" s="3" t="s">
-        <v>789</v>
-      </c>
-      <c r="C2" t="s">
-        <v>791</v>
-      </c>
-      <c r="D2" t="s">
-        <v>792</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>793</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>727</v>
-      </c>
-      <c r="G2" t="s">
-        <v>794</v>
-      </c>
-      <c r="H2" t="s">
-        <v>795</v>
-      </c>
-      <c r="I2" t="s">
-        <v>767</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>748</v>
-      </c>
-      <c r="K2" t="s">
-        <v>796</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{157F74EF-AF50-4C9A-AD23-03F5C2C7CA5B}"/>
-    <hyperlink ref="E2" r:id="rId2" xr:uid="{7C8979B8-4FCF-425E-889B-F1634B71312D}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CDAA5F6-59A5-46C2-91A2-2AB506189DA3}">
-  <dimension ref="A1:N2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="6" max="6" width="12.109375" customWidth="1"/>
-    <col min="7" max="7" width="12" customWidth="1"/>
-    <col min="8" max="8" width="13.77734375" customWidth="1"/>
-    <col min="9" max="9" width="14.109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>798</v>
-      </c>
-      <c r="B1" t="s">
-        <v>797</v>
-      </c>
-      <c r="C1" t="s">
-        <v>799</v>
-      </c>
-      <c r="D1" t="s">
-        <v>800</v>
-      </c>
-      <c r="E1" t="s">
-        <v>801</v>
-      </c>
-      <c r="F1" t="s">
-        <v>802</v>
-      </c>
-      <c r="G1" t="s">
-        <v>803</v>
-      </c>
-      <c r="H1" t="s">
-        <v>804</v>
-      </c>
-      <c r="I1" t="s">
-        <v>805</v>
-      </c>
-      <c r="J1" t="s">
-        <v>806</v>
-      </c>
-      <c r="K1" t="s">
-        <v>807</v>
-      </c>
-      <c r="L1" t="s">
-        <v>808</v>
-      </c>
-      <c r="M1" t="s">
-        <v>809</v>
-      </c>
-      <c r="N1" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>810</v>
-      </c>
-      <c r="B2" t="s">
-        <v>811</v>
-      </c>
-      <c r="C2" t="s">
-        <v>774</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>684</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>696</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>819</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>818</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>812</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>813</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>814</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>683</v>
-      </c>
-      <c r="L2" s="1" t="s">
-        <v>815</v>
-      </c>
-      <c r="M2" s="1" t="s">
-        <v>816</v>
-      </c>
-      <c r="N2" t="s">
-        <v>817</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>